<commit_message>
save all just in case
</commit_message>
<xml_diff>
--- a/data-set/data.xlsx
+++ b/data-set/data.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H379"/>
+  <dimension ref="A1:H381"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A360" sqref="A360:XFD360"/>
@@ -11802,6 +11802,66 @@
         </is>
       </c>
     </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>2021-04-16T05:19:38Z</t>
+        </is>
+      </c>
+      <c r="B380" t="n">
+        <v>71.5</v>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>3324.0</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>2180.0</t>
+        </is>
+      </c>
+      <c r="G380" t="inlineStr">
+        <is>
+          <t>i-0567cbb08247aba69</t>
+        </is>
+      </c>
+      <c r="H380" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>2021-04-16T05:21:39Z</t>
+        </is>
+      </c>
+      <c r="B381" t="n">
+        <v>73.1148</v>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>3422.0</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>2132.0</t>
+        </is>
+      </c>
+      <c r="G381" t="inlineStr">
+        <is>
+          <t>i-0567cbb08247aba69</t>
+        </is>
+      </c>
+      <c r="H381" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>